<commit_message>
Agregando ejemplos de loc
</commit_message>
<xml_diff>
--- a/titanic.xlsx
+++ b/titanic.xlsx
@@ -507,7 +507,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Braund, Mr. Owen Harris</t>
+          <t>anonymous</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -551,7 +551,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Cumings, Mrs. John Bradley (Florence Briggs Thayer)</t>
+          <t>anonymous</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -599,7 +599,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Heikkinen, Miss. Laina</t>
+          <t>anonymous</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">

</xml_diff>